<commit_message>
delete employee date in excel
</commit_message>
<xml_diff>
--- a/uploads/templete_import_users.xlsx
+++ b/uploads/templete_import_users.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Princes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lms_isuzu\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98E7AAA-B34F-42FE-8B3F-0D410B6219AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>No</t>
   </si>
@@ -47,9 +48,6 @@
     <t>Lastname (TH)</t>
   </si>
   <si>
-    <t>Employment date</t>
-  </si>
-  <si>
     <t>KIND</t>
   </si>
   <si>
@@ -90,9 +88,6 @@
   </si>
   <si>
     <t>XXXXX</t>
-  </si>
-  <si>
-    <t>DD/MM/YYYY</t>
   </si>
   <si>
     <t>P</t>
@@ -179,7 +174,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +254,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,16 +531,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.69921875" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,244 +601,229 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="N3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="4" t="s">
+      <c r="P3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="O4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="P4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="N5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="O5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>